<commit_message>
analysing excel sheets and starting to generate csw files instead and plotting
</commit_message>
<xml_diff>
--- a/large_dots_stats.xlsx
+++ b/large_dots_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>File Name</t>
   </si>
@@ -53,6 +53,39 @@
   </si>
   <si>
     <t>eco_filterin_dot\Purine.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\Biosynthesis of amino acids.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\Biosynthesis of cofactors.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\Carbon metabolism.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\Nucleotide metabolism.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\Purine.dot</t>
+  </si>
+  <si>
+    <t>hsa_filtering_dot\test.dot</t>
+  </si>
+  <si>
+    <t>mmu_filtering_dot\Biosynthesis of amino acids.dot</t>
+  </si>
+  <si>
+    <t>mmu_filtering_dot\Biosynthesis of cofactors.dot</t>
+  </si>
+  <si>
+    <t>mmu_filtering_dot\Carbon metabolism.dot</t>
+  </si>
+  <si>
+    <t>mmu_filtering_dot\Nucleotide metabolism.dot</t>
+  </si>
+  <si>
+    <t>mmu_filtering_dot\Purine.dot</t>
   </si>
 </sst>
 </file>
@@ -410,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -572,6 +605,292 @@
         <v>-59.16</v>
       </c>
     </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>434</v>
+      </c>
+      <c r="D7">
+        <v>244</v>
+      </c>
+      <c r="E7">
+        <v>288</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7">
+        <v>-43.78</v>
+      </c>
+      <c r="H7">
+        <v>-65.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>326</v>
+      </c>
+      <c r="C8">
+        <v>886</v>
+      </c>
+      <c r="D8">
+        <v>452</v>
+      </c>
+      <c r="E8">
+        <v>560</v>
+      </c>
+      <c r="F8">
+        <v>126</v>
+      </c>
+      <c r="G8">
+        <v>-48.98</v>
+      </c>
+      <c r="H8">
+        <v>-77.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>181</v>
+      </c>
+      <c r="C9">
+        <v>537</v>
+      </c>
+      <c r="D9">
+        <v>317</v>
+      </c>
+      <c r="E9">
+        <v>356</v>
+      </c>
+      <c r="F9">
+        <v>136</v>
+      </c>
+      <c r="G9">
+        <v>-40.97</v>
+      </c>
+      <c r="H9">
+        <v>-61.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>214</v>
+      </c>
+      <c r="C10">
+        <v>766</v>
+      </c>
+      <c r="D10">
+        <v>468</v>
+      </c>
+      <c r="E10">
+        <v>552</v>
+      </c>
+      <c r="F10">
+        <v>254</v>
+      </c>
+      <c r="G10">
+        <v>-38.9</v>
+      </c>
+      <c r="H10">
+        <v>-53.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>228</v>
+      </c>
+      <c r="C11">
+        <v>772</v>
+      </c>
+      <c r="D11">
+        <v>466</v>
+      </c>
+      <c r="E11">
+        <v>544</v>
+      </c>
+      <c r="F11">
+        <v>238</v>
+      </c>
+      <c r="G11">
+        <v>-39.64</v>
+      </c>
+      <c r="H11">
+        <v>-56.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>-52.94</v>
+      </c>
+      <c r="H12">
+        <v>-85.70999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+      <c r="C13">
+        <v>447</v>
+      </c>
+      <c r="D13">
+        <v>253</v>
+      </c>
+      <c r="E13">
+        <v>297</v>
+      </c>
+      <c r="F13">
+        <v>103</v>
+      </c>
+      <c r="G13">
+        <v>-43.4</v>
+      </c>
+      <c r="H13">
+        <v>-65.31999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>329</v>
+      </c>
+      <c r="C14">
+        <v>894</v>
+      </c>
+      <c r="D14">
+        <v>456</v>
+      </c>
+      <c r="E14">
+        <v>565</v>
+      </c>
+      <c r="F14">
+        <v>127</v>
+      </c>
+      <c r="G14">
+        <v>-48.99</v>
+      </c>
+      <c r="H14">
+        <v>-77.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>181</v>
+      </c>
+      <c r="C15">
+        <v>537</v>
+      </c>
+      <c r="D15">
+        <v>317</v>
+      </c>
+      <c r="E15">
+        <v>356</v>
+      </c>
+      <c r="F15">
+        <v>136</v>
+      </c>
+      <c r="G15">
+        <v>-40.97</v>
+      </c>
+      <c r="H15">
+        <v>-61.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>214</v>
+      </c>
+      <c r="C16">
+        <v>766</v>
+      </c>
+      <c r="D16">
+        <v>468</v>
+      </c>
+      <c r="E16">
+        <v>552</v>
+      </c>
+      <c r="F16">
+        <v>254</v>
+      </c>
+      <c r="G16">
+        <v>-38.9</v>
+      </c>
+      <c r="H16">
+        <v>-53.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>234</v>
+      </c>
+      <c r="C17">
+        <v>789</v>
+      </c>
+      <c r="D17">
+        <v>475</v>
+      </c>
+      <c r="E17">
+        <v>555</v>
+      </c>
+      <c r="F17">
+        <v>241</v>
+      </c>
+      <c r="G17">
+        <v>-39.8</v>
+      </c>
+      <c r="H17">
+        <v>-56.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>